<commit_message>
changed order of variables in contingency table
changed order of variables in contingency table
</commit_message>
<xml_diff>
--- a/datafiles/dNdS/DnDs_4colonies.xlsx
+++ b/datafiles/dNdS/DnDs_4colonies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eloralopez/Documents/SomaticMutations/OfuAug/DnDs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eloralopez/Documents/GitHub/SomMuts/ScriptsandData/datafiles/dNdS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A69D6A-492A-114D-BA35-071F71AB059F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571B9739-8C9A-E247-B207-AAD509C21032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="460" windowWidth="16440" windowHeight="14400" activeTab="3" xr2:uid="{6E1506E6-DF07-6A43-9835-68AF31CF6811}"/>
+    <workbookView xWindow="15960" yWindow="460" windowWidth="16440" windowHeight="14400" activeTab="1" xr2:uid="{6E1506E6-DF07-6A43-9835-68AF31CF6811}"/>
   </bookViews>
   <sheets>
     <sheet name="AH09" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1884,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5AB81C-CA76-B04A-84F7-CB43B03E7DA5}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2238,6 +2239,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f>SUM(A11:A26)/SUM(B11:B26)</f>
+        <v>2.529569892473118</v>
+      </c>
       <c r="D27">
         <v>2.529569892473118</v>
       </c>
@@ -2265,7 +2270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D42B7C5-C365-B545-B297-DB4FCB57E2A5}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C28" workbookViewId="0">
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
@@ -2876,8 +2881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146A7F26-734F-2345-919B-C25EE327C7C3}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
remove LOH with minor allele freq >0, add spectra
-added mutation spectra for LoH and GoH categories

-added chisq tests for LOH and GOH categories

-added a filter to remove any variants that were deemed LOH but had a minor allele frequency > 0 ***this is super important***
</commit_message>
<xml_diff>
--- a/datafiles/dNdS/DnDs_4colonies.xlsx
+++ b/datafiles/dNdS/DnDs_4colonies.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eloralopez/Documents/GitHub/SomMuts/ScriptsandData/datafiles/dNdS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571B9739-8C9A-E247-B207-AAD509C21032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF1F5A1-61F9-FA4A-A127-FC16319E3AA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="460" windowWidth="16440" windowHeight="14400" activeTab="1" xr2:uid="{6E1506E6-DF07-6A43-9835-68AF31CF6811}"/>
+    <workbookView xWindow="15960" yWindow="460" windowWidth="16440" windowHeight="14400" activeTab="2" xr2:uid="{6E1506E6-DF07-6A43-9835-68AF31CF6811}"/>
   </bookViews>
   <sheets>
     <sheet name="AH09" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="AH75" sheetId="2" r:id="rId4"/>
-    <sheet name="AH88" sheetId="3" r:id="rId5"/>
-    <sheet name="AH06" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="AH75" sheetId="2" r:id="rId5"/>
+    <sheet name="AH88" sheetId="3" r:id="rId6"/>
+    <sheet name="AH06" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="125">
   <si>
     <t>Site</t>
   </si>
@@ -384,6 +385,33 @@
   </si>
   <si>
     <t>length*ds</t>
+  </si>
+  <si>
+    <t>LRTs</t>
+  </si>
+  <si>
+    <t>AH75</t>
+  </si>
+  <si>
+    <t>M1 likelihood</t>
+  </si>
+  <si>
+    <t>M2 likelihood</t>
+  </si>
+  <si>
+    <t>Twice the diff</t>
+  </si>
+  <si>
+    <t>M1 df</t>
+  </si>
+  <si>
+    <t>M2 df</t>
+  </si>
+  <si>
+    <t>df difference</t>
+  </si>
+  <si>
+    <t>Significant?</t>
   </si>
 </sst>
 </file>
@@ -1885,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5AB81C-CA76-B04A-84F7-CB43B03E7DA5}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2267,6 +2295,87 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA959817-BDA5-134B-8F25-7E2564F68D2D}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-2338.8488419999999</v>
+      </c>
+      <c r="B5">
+        <v>-2338.8488419999999</v>
+      </c>
+      <c r="C5">
+        <f>2*(A5-B5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <f>B8-A8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D42B7C5-C365-B545-B297-DB4FCB57E2A5}">
   <dimension ref="A1:J54"/>
   <sheetViews>
@@ -2877,7 +2986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146A7F26-734F-2345-919B-C25EE327C7C3}">
   <dimension ref="A1:N13"/>
   <sheetViews>
@@ -3232,7 +3341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12D36D8-675D-A14A-9763-22D7D8CA1F2D}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -3765,7 +3874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3067EC-2CFC-0A4D-A5A4-AEB89157AEEC}">
   <dimension ref="A1:N7"/>
   <sheetViews>

</xml_diff>